<commit_message>
Se hacen nuevas pruebas
</commit_message>
<xml_diff>
--- a/code/resultados-excel.xlsx
+++ b/code/resultados-excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,18 +456,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[PDF][PDF] Medio ambiente</t>
+          <t>[PDF][PDF] Efecto del manejo forestal en la diversidad y composición arbórea de un bosque templado del noroeste de México</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://revista.humanidades.unam.mx/revista_32/revista_32_tema06.pdf</t>
+          <t>https://www.scielo.org.mx/pdf/rcscfa/v19n2/v19n2a2.pdf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>… ambiental.“En dicha cumbre se acordaron medidas para la protección del medio ambiente. 
-… , en el cual se demanda la integración del medio ambiente y el desarrollo económico”. Este …</t>
+          <t>En la presente investigación se evaluó el efecto de las prácticas silvícolas en la diversidad 
+y composición de especies arbóreas de un bosque templado del noroeste de México. Para …</t>
         </is>
       </c>
     </row>
@@ -477,144 +477,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[PDF][PDF] Medio ambiente</t>
+          <t>[PDF][PDF] Componentes químicos y su relación con las actividades biológicas de algunos extractos vegetales</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://we.riseup.net/assets/279881/Problemas+ambientales.pdf</t>
+          <t>https://www.redalyc.org/pdf/863/86314868005.pdf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Medio ambiente … 4 Medio ambiente/José Luis Lezama y Boris Graizbord, coordinadores-1a. 
-ed.--México, DF: El Colegio de México, 2010 429 p.; 22 cm.--… Los temas que se abordan …</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>[PDF][PDF] Medio ambiente y desarrollo</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://repositorio.cepal.org/server/api/core/bitstreams/a799dbd6-22cd-4351-9a8f-83a4270da732/content</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Este documento fue preparado por Ricardo Vicari, consultor de la Unidad de Políticas para 
-el Desarrollo Sostenible de la División de Desarrollo Sostenible y Asentamientos Humanos …</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>[PDF][PDF] Desarrollo y medio ambiente: una mirada a Colombia</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://guao.org/sites/default/files/biblioteca/Desarrollo%20y%20medio%20ambiente%20una%20mirada%20a%20Colombia.pdf</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>… ha afectado y afecta el medio ambiente. En Colombia, como … e influye en el medio ambiente 
-y los recursos naturales. Así, … le estamos dando y daremos al medio ambiente; es nuestra …</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>[PDF][PDF] Medio ambiente urbano</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>https://www.redalyc.org/pdf/1694/169414452002.pdf</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>… Medio Ambiente y Desarrollo, con el propósito de orientar la reflexión conjunta sobre la 
-situación en América Latina respecto de las relaciones entre el ambiente y … temática ambiental a …</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>[PDF][PDF] Vulnerabilidad y medio ambiente</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>https://www.buyteknet.info/fileshare/data/ana_pla_sis_amb/Vul_medio%20ambiente.pdf</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>… entre medio ambiente y sociedad el planteamiento tradicional ha sido el de evaluación 
-de impacto, es decir, se selecciona algo que puede generar cambios en el medio ambiente (…</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>[PDF][PDF] Plásticos y medio ambiente</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>https://www.academia.edu/download/59214400/REVISTA_SOBRE_PLASTICOS20190511-120589-1ic8uu6.pdf</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>… nocivos que acarrean al medio ambiente y por ende a la vida… revolución trascendente para 
-el medio ambiente, y hasta … medio ambiente”, por que aún no se les puede considerar como …</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>[PDF][PDF] Ambiente y el Desarrollo</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>https://archivoteologicogranadino.uloyola.es/rfs/article/download/2810/1355</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>… Los Estados deberán promulgar leyes efectivas sobre el medio ambiente. Las normas 
-ambientales y los objetivos y prioridades en materia de gestión del medio ambiente, deberían …</t>
+          <t>Los aceites esenciales y los extractos vegetales son mezclas complejas de metabolitos 
+secundarios que cubren un amplio espectro de efectos farmacológicos mostrando diversas …</t>
         </is>
       </c>
     </row>

</xml_diff>